<commit_message>
Testdata update and OR file update
</commit_message>
<xml_diff>
--- a/Testdata/ExcludedStudiesPage_Data_PROD.xlsx
+++ b/Testdata/ExcludedStudiesPage_Data_PROD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9661985C-511D-4E6A-B470-C9D29DC184B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B821195F-6B1D-4D0C-9447-CBEC79915A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Economic</t>
   </si>
@@ -61,12 +61,6 @@
     <t>ExcludedStudies_Excel_Files</t>
   </si>
   <si>
-    <t>population_name</t>
-  </si>
-  <si>
-    <t>pop_radio_button</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -137,6 +131,30 @@
   </si>
   <si>
     <t>StandardExcelReport-Takeda-MM Maintenance-Real-world Evidence-2023_</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Population_Radio_button</t>
+  </si>
+  <si>
+    <t>slrtype</t>
+  </si>
+  <si>
+    <t>slrtype_Radio_button</t>
+  </si>
+  <si>
+    <t>Clinical_radio_button</t>
+  </si>
+  <si>
+    <t>Economic_radio_button</t>
+  </si>
+  <si>
+    <t>Quality of Life_radio_button</t>
+  </si>
+  <si>
+    <t>Real-world Evidence_radio_button</t>
   </si>
 </sst>
 </file>
@@ -457,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,146 +487,177 @@
     <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G6" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G7" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G13" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>